<commit_message>
Update remeasure_spring survey bands.xlsx
</commit_message>
<xml_diff>
--- a/resources/field_forms/2020/remeasure_spring survey bands.xlsx
+++ b/resources/field_forms/2020/remeasure_spring survey bands.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erikab\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erikab\Dropbox (Smithsonian)\GitHub\Dendrobands\resources\field_forms\2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D48272AA-4D09-49CD-BFF2-66765D99926C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D4A609-9DB3-46E8-84A6-DAFFDBDBBD56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{971309F3-D5A2-47DE-B10A-A6F9CFFF8F5F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
   <si>
     <t xml:space="preserve">Date: </t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t>measure=19.14 in nov2019</t>
+  </si>
+  <si>
+    <t>intra</t>
+  </si>
+  <si>
+    <t>inra</t>
   </si>
 </sst>
 </file>
@@ -136,15 +142,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -167,13 +179,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,20 +513,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71DE4CA7-4985-4228-8204-7B5F0A5EBBC8}">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="8" max="8" width="10.90625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="24.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -509,13 +534,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -550,7 +575,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>70433</v>
       </c>
@@ -581,7 +606,7 @@
       </c>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>80631</v>
       </c>
@@ -612,7 +637,7 @@
       </c>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>120790</v>
       </c>
@@ -643,7 +668,7 @@
       </c>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>122120</v>
       </c>
@@ -674,7 +699,7 @@
       </c>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>140467</v>
       </c>
@@ -705,7 +730,7 @@
       </c>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>140609</v>
       </c>
@@ -736,7 +761,7 @@
       </c>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>150756</v>
       </c>
@@ -767,7 +792,7 @@
       </c>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>170994</v>
       </c>
@@ -798,8 +823,8 @@
       </c>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="1">
+    <row r="13" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="3">
         <v>172499</v>
       </c>
       <c r="B13" s="1">
@@ -830,9 +855,12 @@
         <v>28</v>
       </c>
       <c r="K13" s="1"/>
-    </row>
-    <row r="14" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="1">
+      <c r="L13" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="3">
         <v>202072</v>
       </c>
       <c r="B14" s="1">
@@ -863,9 +891,12 @@
         <v>29</v>
       </c>
       <c r="K14" s="1"/>
+      <c r="L14" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>